<commit_message>
added AL 2019 data, other small changes
</commit_message>
<xml_diff>
--- a/data/datanotes.xlsx
+++ b/data/datanotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmo2\Desktop\Misc Files and Folders\Fun projects\martingale\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53F8F205-130C-4ADB-8036-EB12A7454F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC2A85E-9E6F-4647-B7C4-84102EF0BF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2778FF9A-4225-410D-9621-8F4D0A9569C8}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t>delete boxscore, road, opp, orig sched, covers date and covers score columns</t>
-  </si>
-  <si>
     <t>game</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>ou</t>
+  </si>
+  <si>
+    <t>delete boxscore, road, opp, orig sched, covers.com date and covers.com score columns</t>
   </si>
 </sst>
 </file>
@@ -460,85 +460,85 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:W1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>22</v>
-      </c>
-      <c r="W1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>